<commit_message>
Agregado nuevo caso de prueba: Validar cupón inválido
</commit_message>
<xml_diff>
--- a/TestCases_eCommerce.xlsx
+++ b/TestCases_eCommerce.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc destock\eCommerce-QA-Tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF5CC3E-3162-45CC-A4D2-C667FE9EF1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -110,13 +116,22 @@
   </si>
   <si>
     <t>Descuento aplicado al total</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>Validar Cupón inválido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar mensaje de error claro </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,13 +194,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -223,7 +246,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -257,6 +280,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -291,9 +315,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,14 +491,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -513,7 +547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -530,7 +564,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -547,7 +581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -564,7 +598,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -579,6 +613,17 @@
       </c>
       <c r="E6" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizo planilla con resultados reales y estados
</commit_message>
<xml_diff>
--- a/TestCases_eCommerce.xlsx
+++ b/TestCases_eCommerce.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc destock\eCommerce-QA-Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF5CC3E-3162-45CC-A4D2-C667FE9EF1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC363D07-8820-45D4-8CA4-72657B612AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1395" yWindow="1965" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -118,13 +118,7 @@
     <t>Descuento aplicado al total</t>
   </si>
   <si>
-    <t>TC06</t>
-  </si>
-  <si>
-    <t>Validar Cupón inválido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mostrar mensaje de error claro </t>
+    <t>Pasó</t>
   </si>
 </sst>
 </file>
@@ -492,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +540,9 @@
       <c r="E2" t="s">
         <v>27</v>
       </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -563,6 +560,12 @@
       <c r="E3" t="s">
         <v>28</v>
       </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -580,6 +583,12 @@
       <c r="E4" t="s">
         <v>29</v>
       </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -597,6 +606,12 @@
       <c r="E5" t="s">
         <v>30</v>
       </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -614,16 +629,11 @@
       <c r="E6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
         <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>